<commit_message>
Add updates from excel
</commit_message>
<xml_diff>
--- a/email.xlsx
+++ b/email.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11865"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11865" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="news" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="updates" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t>newsTitle</t>
   </si>
@@ -38,6 +38,83 @@
   </si>
   <si>
     <t>ttt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>suggest</t>
+  </si>
+  <si>
+    <t>Versions</t>
+  </si>
+  <si>
+    <t>updatesTitle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CVEs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>risk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>c</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>d</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>f</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hello中</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1,3,4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>高</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CVEnumber:CVEurl,2:asdf,3:123123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b:1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>02:222</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -45,7 +122,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -77,6 +154,19 @@
       <family val="2"/>
       <charset val="136"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -100,7 +190,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -108,6 +198,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -406,7 +505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -470,15 +569,189 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="15.75" defaultRowHeight="18.75"/>
+  <cols>
+    <col min="1" max="1" width="15.75" style="3"/>
+    <col min="2" max="2" width="43.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12.75" style="3" customWidth="1"/>
+    <col min="4" max="5" width="12.875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="7.375" style="3" customWidth="1"/>
+    <col min="7" max="16384" width="15.75" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" s="4" customFormat="1">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="5" customFormat="1">
+      <c r="A2" s="5">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5">
+        <v>3</v>
+      </c>
+      <c r="D2" s="5">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5">
+        <v>5</v>
+      </c>
+      <c r="F2" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="5" customFormat="1">
+      <c r="A3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="5" customFormat="1">
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="5" customFormat="1">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="5" customFormat="1">
+      <c r="A6" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="5" customFormat="1">
+      <c r="A7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="5" customFormat="1">
+      <c r="A8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="A3" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add chinese html tag
</commit_message>
<xml_diff>
--- a/email.xlsx
+++ b/email.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>newsTitle</t>
   </si>
@@ -86,35 +86,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>高</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CVEnumber:CVEurl,2:asdf,3:123123</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>b:1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>02:222</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>22</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>b@1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CVEnumber@CVEurl,2@asdf,3@123123</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>02@222</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -569,10 +557,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.75" defaultRowHeight="18.75"/>
@@ -610,7 +598,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2" s="5">
         <v>3</v>
@@ -627,7 +615,7 @@
     </row>
     <row r="3" spans="1:6" s="5" customFormat="1">
       <c r="A3" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>20</v>
@@ -647,7 +635,7 @@
     </row>
     <row r="4" spans="1:6" s="5" customFormat="1">
       <c r="A4" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>20</v>
@@ -670,7 +658,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5" s="5">
         <v>1</v>
@@ -682,66 +670,26 @@
         <v>17</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1">
       <c r="A6" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>13</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="5" customFormat="1">
-      <c r="A7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-      <c r="D7" s="5">
-        <v>1</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="5" customFormat="1">
-      <c r="A8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="5" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>